<commit_message>
Case study finished succussfully
</commit_message>
<xml_diff>
--- a/Case study/Num Res.xlsx
+++ b/Case study/Num Res.xlsx
@@ -5,27 +5,37 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarzaminDigital\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inosoft_04\Desktop\PAPER\MATLAB\Case study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF334B7-FC0D-4FAF-A8AE-8A1BD36C8392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0748FD-C39E-4E4E-B584-417B3F9A8008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="0" windowWidth="16950" windowHeight="10860" xr2:uid="{D6129A20-1F81-494B-BF6B-C0ED5DF90618}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{D6129A20-1F81-494B-BF6B-C0ED5DF90618}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Entropy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="26">
   <si>
     <t>NSGA-II</t>
   </si>
@@ -53,12 +63,66 @@
   <si>
     <t>QM</t>
   </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>npop=30</t>
+  </si>
+  <si>
+    <t>npop=50</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>r_ij</t>
+  </si>
+  <si>
+    <t>MOEA/D</t>
+  </si>
+  <si>
+    <t>PESA-II</t>
+  </si>
+  <si>
+    <t>h=</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>e_j=</t>
+  </si>
+  <si>
+    <t>1-e_j=</t>
+  </si>
+  <si>
+    <t>w_j=</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,8 +145,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,8 +179,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,11 +206,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -137,6 +236,53 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA82E70-FE4C-4668-AB26-ACA18349451D}">
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,837 +632,921 @@
     <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="G1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="L1" s="4" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="L1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="Q1" s="4" t="s">
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="Q1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="V1" s="5" t="s">
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="V1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="AA1" s="4" t="s">
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="AA1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="T2" s="7"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="X2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AB2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AC2" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE2" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="7">
         <v>83</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="7">
         <v>29</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="7">
         <v>49</v>
       </c>
-      <c r="F3" s="2">
+      <c r="E3" s="7"/>
+      <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="7">
         <v>0.71531</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="7">
         <v>0.84175999999999995</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="7">
         <v>0.83125000000000004</v>
       </c>
-      <c r="K3" s="2">
+      <c r="J3" s="7"/>
+      <c r="K3" s="6">
         <v>1</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="7">
         <v>2159.0895</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="7">
         <v>1865.8181</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="7">
         <v>2142.4690000000001</v>
       </c>
-      <c r="P3" s="2">
+      <c r="O3" s="7"/>
+      <c r="P3" s="6">
         <v>1</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="Q3" s="7">
         <v>0.25280000000000002</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="7">
         <v>0.25081999999999999</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" s="7">
         <v>0.19431000000000001</v>
       </c>
-      <c r="U3" s="2">
+      <c r="T3" s="7"/>
+      <c r="U3" s="6">
         <v>1</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3" s="7">
         <v>133.7747</v>
       </c>
-      <c r="W3" s="1">
+      <c r="W3" s="7">
         <v>114.0697</v>
       </c>
-      <c r="X3" s="1">
+      <c r="X3" s="7">
         <v>127.7285</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="6">
         <v>1</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AA3" s="7">
         <v>0.38550000000000001</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AB3" s="7">
         <v>0</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AC3" s="7">
         <v>0.91839999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="10"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="7">
         <v>78</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="7">
         <v>25</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="7">
         <v>62</v>
       </c>
-      <c r="F4" s="2">
+      <c r="E4" s="7"/>
+      <c r="F4" s="6">
         <v>2</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="7">
         <v>0.68645</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="7">
         <v>0.89222000000000001</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="7">
         <v>0.84219999999999995</v>
       </c>
-      <c r="K4" s="2">
+      <c r="J4" s="7"/>
+      <c r="K4" s="6">
         <v>2</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="7">
         <v>4421.0258000000003</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="7">
         <v>2024.6110000000001</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="7">
         <v>3693.8163</v>
       </c>
-      <c r="P4" s="2">
+      <c r="O4" s="7"/>
+      <c r="P4" s="6">
         <v>2</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="7">
         <v>0.22799</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="7">
         <v>0.27528000000000002</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4" s="7">
         <v>0.18618000000000001</v>
       </c>
-      <c r="U4" s="2">
+      <c r="T4" s="7"/>
+      <c r="U4" s="6">
         <v>2</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4" s="7">
         <v>124.8781</v>
       </c>
-      <c r="W4" s="1">
+      <c r="W4" s="7">
         <v>94.115499999999997</v>
       </c>
-      <c r="X4" s="1">
+      <c r="X4" s="7">
         <v>114.7376</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="6">
         <v>2</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AA4" s="7">
         <v>0.89739999999999998</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="7">
         <v>0.32</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AC4" s="7">
         <v>0.30649999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="10"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="7">
         <v>91</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="7">
         <v>30</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="7">
         <v>65</v>
       </c>
-      <c r="F5" s="2">
+      <c r="E5" s="7"/>
+      <c r="F5" s="6">
         <v>3</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="7">
         <v>0.79224000000000006</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="7">
         <v>0.90185999999999999</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="7">
         <v>0.82979999999999998</v>
       </c>
-      <c r="K5" s="2">
+      <c r="J5" s="7"/>
+      <c r="K5" s="6">
         <v>3</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="7">
         <v>3005.2703000000001</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="7">
         <v>1784.9319</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="7">
         <v>1947.9908</v>
       </c>
-      <c r="P5" s="2">
+      <c r="O5" s="7"/>
+      <c r="P5" s="6">
         <v>3</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="Q5" s="7">
         <v>0.30785000000000001</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="7">
         <v>0.15060000000000001</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="7">
         <v>0.22886000000000001</v>
       </c>
-      <c r="U5" s="2">
+      <c r="T5" s="7"/>
+      <c r="U5" s="6">
         <v>3</v>
       </c>
-      <c r="V5" s="1">
+      <c r="V5" s="7">
         <v>130.99449999999999</v>
       </c>
-      <c r="W5" s="1">
+      <c r="W5" s="7">
         <v>112.4606</v>
       </c>
-      <c r="X5" s="1">
+      <c r="X5" s="7">
         <v>113.86790000000001</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="6">
         <v>3</v>
       </c>
-      <c r="AA5" s="1">
+      <c r="AA5" s="7">
         <v>1</v>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5" s="7">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="AC5" s="1">
+      <c r="AC5" s="7">
         <v>0.23080000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="10"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="7">
         <v>95</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="7">
         <v>30</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="7">
         <v>38</v>
       </c>
-      <c r="F6" s="2">
+      <c r="E6" s="7"/>
+      <c r="F6" s="6">
         <v>4</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="7">
         <v>0.87977000000000005</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="7">
         <v>0.84211999999999998</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="7">
         <v>1.0079</v>
       </c>
-      <c r="K6" s="2">
+      <c r="J6" s="7"/>
+      <c r="K6" s="6">
         <v>4</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="7">
         <v>2428.1095</v>
       </c>
-      <c r="M6" s="1">
+      <c r="M6" s="7">
         <v>1967.7083</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="7">
         <v>1558.683</v>
       </c>
-      <c r="P6" s="2">
+      <c r="O6" s="7"/>
+      <c r="P6" s="6">
         <v>4</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="7">
         <v>0.2422</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="7">
         <v>0.25535999999999998</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="7">
         <v>0.22148999999999999</v>
       </c>
-      <c r="U6" s="2">
+      <c r="T6" s="7"/>
+      <c r="U6" s="6">
         <v>4</v>
       </c>
-      <c r="V6" s="1">
+      <c r="V6" s="7">
         <v>118.30500000000001</v>
       </c>
-      <c r="W6" s="1">
+      <c r="W6" s="7">
         <v>118.8655</v>
       </c>
-      <c r="X6" s="1">
+      <c r="X6" s="7">
         <v>127.37569999999999</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="6">
         <v>4</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AA6" s="7">
         <v>0.75790000000000002</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="7">
         <v>0.2</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AC6" s="7">
         <v>0.52629999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="10"/>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="7">
         <v>101</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="7">
         <v>30</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="7">
         <v>38</v>
       </c>
-      <c r="F7" s="2">
+      <c r="E7" s="7"/>
+      <c r="F7" s="6">
         <v>5</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="7">
         <v>0.97928000000000004</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="7">
         <v>0.82143999999999995</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="7">
         <v>0.87290000000000001</v>
       </c>
-      <c r="K7" s="2">
+      <c r="J7" s="7"/>
+      <c r="K7" s="6">
         <v>5</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="7">
         <v>2438.5095999999999</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="7">
         <v>1829.2913000000001</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="7">
         <v>997.45309999999995</v>
       </c>
-      <c r="P7" s="2">
+      <c r="O7" s="7"/>
+      <c r="P7" s="6">
         <v>5</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7" s="7">
         <v>0.22864999999999999</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="7">
         <v>0.26228000000000001</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="7">
         <v>0.16342999999999999</v>
       </c>
-      <c r="U7" s="2">
+      <c r="T7" s="7"/>
+      <c r="U7" s="6">
         <v>5</v>
       </c>
-      <c r="V7" s="1">
+      <c r="V7" s="7">
         <v>155.76070000000001</v>
       </c>
-      <c r="W7" s="1">
+      <c r="W7" s="7">
         <v>116.3004</v>
       </c>
-      <c r="X7" s="1">
+      <c r="X7" s="7">
         <v>101.7307</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="6">
         <v>5</v>
       </c>
-      <c r="AA7" s="1">
+      <c r="AA7" s="7">
         <v>0.85150000000000003</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="7">
         <v>0.5333</v>
       </c>
-      <c r="AC7" s="1">
+      <c r="AC7" s="7">
         <v>0.89470000000000005</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="10"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="7">
         <v>97</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="7">
         <v>27</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="7">
         <v>70</v>
       </c>
-      <c r="F8" s="2">
+      <c r="E8" s="7"/>
+      <c r="F8" s="6">
         <v>6</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="7">
         <v>0.72148000000000001</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="7">
         <v>0.92752000000000001</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="7">
         <v>0.80662999999999996</v>
       </c>
-      <c r="K8" s="2">
+      <c r="J8" s="7"/>
+      <c r="K8" s="6">
         <v>6</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="7">
         <v>5587.2249000000002</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="7">
         <v>1909.9447</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="7">
         <v>2691.6351</v>
       </c>
-      <c r="P8" s="2">
+      <c r="O8" s="7"/>
+      <c r="P8" s="6">
         <v>6</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="7">
         <v>0.36359000000000002</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="7">
         <v>0.20702000000000001</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8" s="7">
         <v>0.21911</v>
       </c>
-      <c r="U8" s="2">
+      <c r="T8" s="7"/>
+      <c r="U8" s="6">
         <v>6</v>
       </c>
-      <c r="V8" s="1">
+      <c r="V8" s="7">
         <v>153.21899999999999</v>
       </c>
-      <c r="W8" s="1">
+      <c r="W8" s="7">
         <v>116.6992</v>
       </c>
-      <c r="X8" s="1">
+      <c r="X8" s="7">
         <v>122.64149999999999</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="6">
         <v>6</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AA8" s="7">
         <v>0.97940000000000005</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AB8" s="7">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AC8" s="7">
         <v>0.15709999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="10"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="7">
         <v>53</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="7">
         <v>25</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="7">
         <v>92</v>
       </c>
-      <c r="F9" s="2">
+      <c r="E9" s="7"/>
+      <c r="F9" s="6">
         <v>7</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="7">
         <v>0.64549999999999996</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="7">
         <v>0.75000999999999995</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="7">
         <v>0.80174999999999996</v>
       </c>
-      <c r="K9" s="2">
+      <c r="J9" s="7"/>
+      <c r="K9" s="6">
         <v>7</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="7">
         <v>2237.9157</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="7">
         <v>1829.1008999999999</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="7">
         <v>2555.4976000000001</v>
       </c>
-      <c r="P9" s="2">
+      <c r="O9" s="7"/>
+      <c r="P9" s="6">
         <v>7</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="7">
         <v>0.17332</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="7">
         <v>0.31789000000000001</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9" s="7">
         <v>0.18268999999999999</v>
       </c>
-      <c r="U9" s="2">
+      <c r="T9" s="7"/>
+      <c r="U9" s="6">
         <v>7</v>
       </c>
-      <c r="V9" s="1">
+      <c r="V9" s="7">
         <v>122.5583</v>
       </c>
-      <c r="W9" s="1">
+      <c r="W9" s="7">
         <v>125.7059</v>
       </c>
-      <c r="X9" s="1">
+      <c r="X9" s="7">
         <v>119.1268</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="6">
         <v>7</v>
       </c>
-      <c r="AA9" s="1">
+      <c r="AA9" s="7">
         <v>0.94340000000000002</v>
       </c>
-      <c r="AB9" s="1">
+      <c r="AB9" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AC9" s="7">
         <v>0.1196</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD9" s="12"/>
+      <c r="AE9" s="10"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="7">
         <v>77</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="7">
         <v>26</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="7">
         <v>31</v>
       </c>
-      <c r="F10" s="2">
+      <c r="E10" s="7"/>
+      <c r="F10" s="6">
         <v>8</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="7">
         <v>0.82174000000000003</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="7">
         <v>0.77508999999999995</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="7">
         <v>1.0820000000000001</v>
       </c>
-      <c r="K10" s="2">
+      <c r="J10" s="7"/>
+      <c r="K10" s="6">
         <v>8</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="7">
         <v>1839.3648000000001</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="7">
         <v>1632.8586</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="7">
         <v>2763.3577</v>
       </c>
-      <c r="P10" s="2">
+      <c r="O10" s="7"/>
+      <c r="P10" s="6">
         <v>8</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="Q10" s="7">
         <v>0.31225999999999998</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="7">
         <v>0.28226000000000001</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10" s="7">
         <v>0.19300999999999999</v>
       </c>
-      <c r="U10" s="2">
+      <c r="T10" s="7"/>
+      <c r="U10" s="6">
         <v>8</v>
       </c>
-      <c r="V10" s="1">
+      <c r="V10" s="7">
         <v>136.57220000000001</v>
       </c>
-      <c r="W10" s="1">
+      <c r="W10" s="7">
         <v>128.9699</v>
       </c>
-      <c r="X10" s="1">
+      <c r="X10" s="7">
         <v>152.55189999999999</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="6">
         <v>8</v>
       </c>
-      <c r="AA10" s="1">
+      <c r="AA10" s="7">
         <v>0.74029999999999996</v>
       </c>
-      <c r="AB10" s="1">
+      <c r="AB10" s="7">
         <v>0.1923</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AC10" s="7">
         <v>0.3871</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="10"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="7">
         <v>34</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="7">
         <v>26</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="7">
         <v>46</v>
       </c>
-      <c r="F11" s="2">
+      <c r="E11" s="7"/>
+      <c r="F11" s="6">
         <v>9</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="7">
         <v>0.84157000000000004</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="7">
         <v>0.91464999999999996</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="7">
         <v>0.75241999999999998</v>
       </c>
-      <c r="K11" s="2">
+      <c r="J11" s="7"/>
+      <c r="K11" s="6">
         <v>9</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="7">
         <v>2460.1030000000001</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="7">
         <v>1801.0408</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="7">
         <v>1941.7731000000001</v>
       </c>
-      <c r="P11" s="2">
+      <c r="O11" s="7"/>
+      <c r="P11" s="6">
         <v>9</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Q11" s="7">
         <v>0.28037000000000001</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="7">
         <v>0.17019999999999999</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" s="7">
         <v>0.21793000000000001</v>
       </c>
-      <c r="U11" s="2">
+      <c r="T11" s="7"/>
+      <c r="U11" s="6">
         <v>9</v>
       </c>
-      <c r="V11" s="1">
+      <c r="V11" s="7">
         <v>134.86019999999999</v>
       </c>
-      <c r="W11" s="1">
+      <c r="W11" s="7">
         <v>121.7064</v>
       </c>
-      <c r="X11" s="1">
+      <c r="X11" s="7">
         <v>133.21369999999999</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="6">
         <v>9</v>
       </c>
-      <c r="AA11" s="1">
+      <c r="AA11" s="7">
         <v>0.47060000000000002</v>
       </c>
-      <c r="AB11" s="1">
+      <c r="AB11" s="7">
         <v>0.46150000000000002</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AC11" s="7">
         <v>0.19570000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="10"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="7">
         <v>60</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="7">
         <v>29</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="7">
         <v>41</v>
       </c>
-      <c r="F12" s="2">
+      <c r="E12" s="7"/>
+      <c r="F12" s="6">
         <v>10</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="7">
         <v>0.82396999999999998</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="7">
         <v>0.88934999999999997</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="7">
         <v>0.90663000000000005</v>
       </c>
-      <c r="K12" s="2">
+      <c r="J12" s="7"/>
+      <c r="K12" s="6">
         <v>10</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="7">
         <v>2191.8798999999999</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="7">
         <v>3154.1939000000002</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="7">
         <v>1510.7166999999999</v>
       </c>
-      <c r="P12" s="2">
+      <c r="O12" s="7"/>
+      <c r="P12" s="6">
         <v>10</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="Q12" s="7">
         <v>0.19599</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R12" s="7">
         <v>0.24364</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S12" s="7">
         <v>0.17204</v>
       </c>
-      <c r="U12" s="2">
+      <c r="T12" s="7"/>
+      <c r="U12" s="6">
         <v>10</v>
       </c>
-      <c r="V12" s="1">
+      <c r="V12" s="7">
         <v>134.6978</v>
       </c>
-      <c r="W12" s="1">
+      <c r="W12" s="7">
         <v>119.35169999999999</v>
       </c>
-      <c r="X12" s="1">
+      <c r="X12" s="7">
         <v>117.32089999999999</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="6">
         <v>10</v>
       </c>
-      <c r="AA12" s="1">
+      <c r="AA12" s="7">
         <v>0.86670000000000003</v>
       </c>
-      <c r="AB12" s="1">
+      <c r="AB12" s="7">
         <v>0.51719999999999999</v>
       </c>
-      <c r="AC12" s="1">
+      <c r="AC12" s="7">
         <v>0.439</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD12" s="12"/>
+      <c r="AE12" s="10"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f>SUM(B3:B12)/10</f>
         <v>76.900000000000006</v>
@@ -1390,16 +1620,1366 @@
         <v>0.41751999999999995</v>
       </c>
     </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="G15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="L15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="Q15" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="V15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="AA15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+      <c r="AE15" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>83</v>
+      </c>
+      <c r="C16" s="1">
+        <v>29</v>
+      </c>
+      <c r="D16" s="1">
+        <v>73</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.71531</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.84175999999999995</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.84611000000000003</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2159.0895</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1865.8181</v>
+      </c>
+      <c r="N16" s="1">
+        <v>2694.9195</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0.25280000000000002</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0.25081999999999999</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0.26843</v>
+      </c>
+      <c r="V16" s="1">
+        <v>133.7747</v>
+      </c>
+      <c r="W16" s="1">
+        <v>114.0697</v>
+      </c>
+      <c r="X16" s="1">
+        <v>135.10380000000001</v>
+      </c>
+      <c r="AA16" s="1">
+        <v>8.43E-2</v>
+      </c>
+      <c r="AB16" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="10"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1">
+        <v>78</v>
+      </c>
+      <c r="C17" s="1">
+        <v>25</v>
+      </c>
+      <c r="D17" s="1">
+        <v>57</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.68645</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.89222000000000001</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.64768999999999999</v>
+      </c>
+      <c r="L17" s="1">
+        <v>4421.0258000000003</v>
+      </c>
+      <c r="M17" s="1">
+        <v>2024.6110000000001</v>
+      </c>
+      <c r="N17" s="1">
+        <v>4918.8171000000002</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0.22799</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0.27528000000000002</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0.30436999999999997</v>
+      </c>
+      <c r="V17" s="1">
+        <v>124.8781</v>
+      </c>
+      <c r="W17" s="1">
+        <v>94.115499999999997</v>
+      </c>
+      <c r="X17" s="1">
+        <v>137.61930000000001</v>
+      </c>
+      <c r="AA17" s="1">
+        <v>0.17949999999999999</v>
+      </c>
+      <c r="AB17" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>0.85960000000000003</v>
+      </c>
+      <c r="AE17" s="10"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>91</v>
+      </c>
+      <c r="C18" s="1">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1">
+        <v>57</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.79224000000000006</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.90185999999999999</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.92571000000000003</v>
+      </c>
+      <c r="L18" s="1">
+        <v>3005.2703000000001</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1784.9319</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1884.6762000000001</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0.30785000000000001</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0.15060000000000001</v>
+      </c>
+      <c r="S18" s="1">
+        <v>0.20827999999999999</v>
+      </c>
+      <c r="V18" s="1">
+        <v>130.99449999999999</v>
+      </c>
+      <c r="W18" s="1">
+        <v>112.4606</v>
+      </c>
+      <c r="X18" s="1">
+        <v>130.73330000000001</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>0.29670000000000002</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="1">
+        <v>0.77190000000000003</v>
+      </c>
+      <c r="AE18" s="10"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>95</v>
+      </c>
+      <c r="C19" s="1">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1">
+        <v>68</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.87977000000000005</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.84211999999999998</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.76780000000000004</v>
+      </c>
+      <c r="L19" s="1">
+        <v>2428.1095</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1967.7083</v>
+      </c>
+      <c r="N19" s="1">
+        <v>2752.7420000000002</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>0.2422</v>
+      </c>
+      <c r="R19" s="1">
+        <v>0.25535999999999998</v>
+      </c>
+      <c r="S19" s="1">
+        <v>0.28903000000000001</v>
+      </c>
+      <c r="V19" s="1">
+        <v>118.30500000000001</v>
+      </c>
+      <c r="W19" s="1">
+        <v>118.8655</v>
+      </c>
+      <c r="X19" s="1">
+        <v>112.8603</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>0.21049999999999999</v>
+      </c>
+      <c r="AB19" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="1">
+        <v>0.86760000000000004</v>
+      </c>
+      <c r="AE19" s="10"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1">
+        <v>101</v>
+      </c>
+      <c r="C20" s="1">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1">
+        <v>72</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.97928000000000004</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.82143999999999995</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.90347999999999995</v>
+      </c>
+      <c r="L20" s="1">
+        <v>2438.5095999999999</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1829.2913000000001</v>
+      </c>
+      <c r="N20" s="1">
+        <v>1135.2553</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0.22864999999999999</v>
+      </c>
+      <c r="R20" s="1">
+        <v>0.26228000000000001</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0.16850000000000001</v>
+      </c>
+      <c r="V20" s="1">
+        <v>155.76070000000001</v>
+      </c>
+      <c r="W20" s="1">
+        <v>116.3004</v>
+      </c>
+      <c r="X20" s="1">
+        <v>118.3715</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>0.6139</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="AE20" s="10"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1">
+        <v>97</v>
+      </c>
+      <c r="C21" s="1">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1">
+        <v>80</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.72148000000000001</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.92752000000000001</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.98246999999999995</v>
+      </c>
+      <c r="L21" s="1">
+        <v>5587.2249000000002</v>
+      </c>
+      <c r="M21" s="1">
+        <v>1909.9447</v>
+      </c>
+      <c r="N21" s="1">
+        <v>2729.6583000000001</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>0.36359000000000002</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0.20702000000000001</v>
+      </c>
+      <c r="S21" s="1">
+        <v>0.21135999999999999</v>
+      </c>
+      <c r="V21" s="1">
+        <v>153.21899999999999</v>
+      </c>
+      <c r="W21" s="1">
+        <v>116.6992</v>
+      </c>
+      <c r="X21" s="1">
+        <v>149.60929999999999</v>
+      </c>
+      <c r="AA21" s="1">
+        <v>0.75260000000000005</v>
+      </c>
+      <c r="AB21" s="1">
+        <v>7.4099999999999999E-2</v>
+      </c>
+      <c r="AC21" s="1">
+        <v>0.66249999999999998</v>
+      </c>
+      <c r="AE21" s="10"/>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>7</v>
+      </c>
+      <c r="B22" s="1">
+        <v>53</v>
+      </c>
+      <c r="C22" s="1">
+        <v>25</v>
+      </c>
+      <c r="D22" s="1">
+        <v>80</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0.64549999999999996</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.75000999999999995</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.95384999999999998</v>
+      </c>
+      <c r="L22" s="1">
+        <v>2237.9157</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1829.1008999999999</v>
+      </c>
+      <c r="N22" s="1">
+        <v>2646.7008000000001</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>0.17332</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0.31789000000000001</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0.14102999999999999</v>
+      </c>
+      <c r="V22" s="1">
+        <v>122.5583</v>
+      </c>
+      <c r="W22" s="1">
+        <v>125.7059</v>
+      </c>
+      <c r="X22" s="1">
+        <v>165.0523</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>0.433</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="AC22" s="1">
+        <v>0.95</v>
+      </c>
+      <c r="AE22" s="10"/>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>8</v>
+      </c>
+      <c r="B23" s="1">
+        <v>77</v>
+      </c>
+      <c r="C23" s="1">
+        <v>26</v>
+      </c>
+      <c r="D23" s="1">
+        <v>55</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.82174000000000003</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0.77508999999999995</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.72158999999999995</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1839.3648000000001</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1632.8586</v>
+      </c>
+      <c r="N23" s="1">
+        <v>2429.8885</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0.31225999999999998</v>
+      </c>
+      <c r="R23" s="1">
+        <v>0.28226000000000001</v>
+      </c>
+      <c r="S23" s="1">
+        <v>0.17161999999999999</v>
+      </c>
+      <c r="V23" s="1">
+        <v>136.57220000000001</v>
+      </c>
+      <c r="W23" s="1">
+        <v>128.9699</v>
+      </c>
+      <c r="X23" s="1">
+        <v>123.0697</v>
+      </c>
+      <c r="AA23" s="1">
+        <v>0.46750000000000003</v>
+      </c>
+      <c r="AB23" s="1">
+        <v>0.15379999999999999</v>
+      </c>
+      <c r="AC23" s="1">
+        <v>0.5091</v>
+      </c>
+      <c r="AE23" s="10"/>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1">
+        <v>34</v>
+      </c>
+      <c r="C24" s="1">
+        <v>26</v>
+      </c>
+      <c r="D24" s="1">
+        <v>92</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.84157000000000004</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.91464999999999996</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.98346999999999996</v>
+      </c>
+      <c r="L24" s="1">
+        <v>2460.1030000000001</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1801.0408</v>
+      </c>
+      <c r="N24" s="1">
+        <v>3179.9115999999999</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>0.28037000000000001</v>
+      </c>
+      <c r="R24" s="1">
+        <v>0.17019999999999999</v>
+      </c>
+      <c r="S24" s="1">
+        <v>0.24931</v>
+      </c>
+      <c r="V24" s="1">
+        <v>134.86019999999999</v>
+      </c>
+      <c r="W24" s="1">
+        <v>121.7064</v>
+      </c>
+      <c r="X24" s="1">
+        <v>135.3295</v>
+      </c>
+      <c r="AA24" s="1">
+        <v>0.35289999999999999</v>
+      </c>
+      <c r="AB24" s="1">
+        <v>0.30769999999999997</v>
+      </c>
+      <c r="AC24" s="1">
+        <v>0.9022</v>
+      </c>
+      <c r="AE24" s="10"/>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1">
+        <v>60</v>
+      </c>
+      <c r="C25" s="1">
+        <v>29</v>
+      </c>
+      <c r="D25" s="1">
+        <v>88</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.82396999999999998</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0.88934999999999997</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.878</v>
+      </c>
+      <c r="L25" s="1">
+        <v>2191.8798999999999</v>
+      </c>
+      <c r="M25" s="1">
+        <v>3154.1939000000002</v>
+      </c>
+      <c r="N25" s="1">
+        <v>2378.8254999999999</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>0.19599</v>
+      </c>
+      <c r="R25" s="1">
+        <v>0.24364</v>
+      </c>
+      <c r="S25" s="1">
+        <v>0.20513999999999999</v>
+      </c>
+      <c r="V25" s="1">
+        <v>134.6978</v>
+      </c>
+      <c r="W25" s="1">
+        <v>119.35169999999999</v>
+      </c>
+      <c r="X25" s="1">
+        <v>148.17420000000001</v>
+      </c>
+      <c r="AA25" s="1">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="AB25" s="1">
+        <v>0.51719999999999999</v>
+      </c>
+      <c r="AC25" s="1">
+        <v>0.59089999999999998</v>
+      </c>
+      <c r="AE25" s="10"/>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B26" s="8">
+        <f>SUM(B16:B25)/10</f>
+        <v>76.900000000000006</v>
+      </c>
+      <c r="C26" s="8">
+        <f t="shared" ref="C26:AC26" si="1">SUM(C16:C25)/10</f>
+        <v>27.7</v>
+      </c>
+      <c r="D26" s="8">
+        <f t="shared" si="1"/>
+        <v>72.2</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.79073099999999996</v>
+      </c>
+      <c r="H26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.85560199999999997</v>
+      </c>
+      <c r="I26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.86101700000000003</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" s="8">
+        <f t="shared" si="1"/>
+        <v>2876.8493000000003</v>
+      </c>
+      <c r="M26" s="8">
+        <f t="shared" si="1"/>
+        <v>1979.9499499999997</v>
+      </c>
+      <c r="N26" s="8">
+        <f t="shared" si="1"/>
+        <v>2675.1394799999998</v>
+      </c>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.25850200000000001</v>
+      </c>
+      <c r="R26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.241535</v>
+      </c>
+      <c r="S26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22170700000000002</v>
+      </c>
+      <c r="U26" s="1"/>
+      <c r="V26" s="8">
+        <f t="shared" si="1"/>
+        <v>134.56205</v>
+      </c>
+      <c r="W26" s="8">
+        <f t="shared" si="1"/>
+        <v>116.82447999999999</v>
+      </c>
+      <c r="X26" s="8">
+        <f t="shared" si="1"/>
+        <v>135.59232</v>
+      </c>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.40576000000000001</v>
+      </c>
+      <c r="AB26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.16831000000000002</v>
+      </c>
+      <c r="AC26" s="8">
+        <f t="shared" si="1"/>
+        <v>0.78637999999999997</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="15">
+    <mergeCell ref="AD2:AD12"/>
+    <mergeCell ref="AE2:AE12"/>
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="V1:X1"/>
+    <mergeCell ref="AA15:AC15"/>
+    <mergeCell ref="AE15:AE25"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="V15:X15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB4218F-2606-4969-8B7B-6617CAB0479F}">
+  <dimension ref="B1:AH9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AE11" sqref="AE11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="9" max="9" width="2.140625" customWidth="1"/>
+    <col min="16" max="16" width="2.85546875" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="17">
+        <f>1/LN(3)</f>
+        <v>0.91023922662683732</v>
+      </c>
+      <c r="AD1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.79073099999999996</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2876.8493000000003</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.25850200000000001</v>
+      </c>
+      <c r="G3" s="1">
+        <v>134.56205</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.40576000000000001</v>
+      </c>
+      <c r="J3" s="1">
+        <f>(C3-C$7)/(C$8-C$7)</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
+        <f>(D$8-D3)/(D$8-D$7)</f>
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
+        <f>(E3-E$7)/(E$8-E$7)</f>
+        <v>1</v>
+      </c>
+      <c r="M3" s="1">
+        <f>(F3-F$7)/(F$8-F$7)</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <f>(G$8-G3)/(G$8-G$7)</f>
+        <v>5.4895502092942035E-2</v>
+      </c>
+      <c r="O3" s="1">
+        <f>(H3-H$7)/(H$8-H$7)</f>
+        <v>0.38417978546119375</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>SQRT(J3+K3^2+L3+M3+N3^2+O3^2)</f>
+        <v>2.0373040086612124</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="15">
+        <f>C3/$C$6</f>
+        <v>0.43495475113122173</v>
+      </c>
+      <c r="U3" s="15">
+        <f>D3/$D$6</f>
+        <v>0.31536522623486951</v>
+      </c>
+      <c r="V3" s="15">
+        <f>E3/$E$6</f>
+        <v>0.38195335930461033</v>
+      </c>
+      <c r="W3" s="15">
+        <f>F3/$F$6</f>
+        <v>0.35816300516526633</v>
+      </c>
+      <c r="X3" s="15">
+        <f>G3/$G$6</f>
+        <v>0.34772455910704164</v>
+      </c>
+      <c r="Y3" s="15">
+        <f>H3/$H$6</f>
+        <v>0.29825425410709688</v>
+      </c>
+      <c r="AA3">
+        <f>T3*LN(T3)</f>
+        <v>-0.36210560377211848</v>
+      </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AF5" si="0">U3*LN(U3)</f>
+        <v>-0.36393899677198266</v>
+      </c>
+      <c r="AC3">
+        <f t="shared" si="0"/>
+        <v>-0.36761359797319193</v>
+      </c>
+      <c r="AD3">
+        <f t="shared" si="0"/>
+        <v>-0.36774998101419282</v>
+      </c>
+      <c r="AE3">
+        <f t="shared" si="0"/>
+        <v>-0.36731696357758076</v>
+      </c>
+      <c r="AF3">
+        <f t="shared" si="0"/>
+        <v>-0.36083066734982788</v>
+      </c>
+    </row>
+    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>27.7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.85560199999999997</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1979.9499499999997</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.241535</v>
+      </c>
+      <c r="G4" s="1">
+        <v>116.82447999999999</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.16831000000000002</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:J5" si="1">(C4-C$7)/(C$8-C$7)</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K5" si="2">(D$8-D4)/(D$8-D$7)</f>
+        <v>7.7042369746465209E-2</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" ref="L4:M5" si="3">(E4-E$7)/(E$8-E$7)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" si="3"/>
+        <v>0.53887756488653316</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N5" si="4">(G$8-G4)/(G$8-G$7)</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" ref="O4:O5" si="5">(H4-H$7)/(H$8-H$7)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ref="Q4:Q5" si="6">SQRT(J4+K4^2+L4+M4+N4^2+O4^2)</f>
+        <v>1.242905101615841</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T4" s="15">
+        <f t="shared" ref="T4:T5" si="7">C4/$C$6</f>
+        <v>0.15667420814479638</v>
+      </c>
+      <c r="U4" s="15">
+        <f t="shared" ref="U4:U5" si="8">D4/$D$6</f>
+        <v>0.34123756156898721</v>
+      </c>
+      <c r="V4" s="15">
+        <f t="shared" ref="V4:V5" si="9">E4/$E$6</f>
+        <v>0.26287387895413744</v>
+      </c>
+      <c r="W4" s="15">
+        <f t="shared" ref="W4:W5" si="10">F4/$F$6</f>
+        <v>0.33465466979981817</v>
+      </c>
+      <c r="X4" s="15">
+        <f t="shared" ref="X4:X5" si="11">G4/$G$6</f>
+        <v>0.30188853990340819</v>
+      </c>
+      <c r="Y4" s="15">
+        <f t="shared" ref="Y4:Y5" si="12">H4/$H$6</f>
+        <v>0.12371641736190231</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" ref="AA4:AA5" si="13">T4*LN(T4)</f>
+        <v>-0.2904092342487779</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="0"/>
+        <v>-0.36689056711025547</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" si="0"/>
+        <v>-0.35122077128394619</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" si="0"/>
+        <v>-0.3663317807942767</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" si="0"/>
+        <v>-0.36157112020729937</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" si="0"/>
+        <v>-0.25853802727616293</v>
+      </c>
+    </row>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>72.2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.86101700000000003</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2675.1394799999998</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.22170700000000002</v>
+      </c>
+      <c r="G5" s="1">
+        <v>135.59232</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.78637999999999997</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>0.90447154471544711</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.77510317071809631</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="6"/>
+        <v>1.6369406572730556</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T5" s="15">
+        <f t="shared" si="7"/>
+        <v>0.40837104072398189</v>
+      </c>
+      <c r="U5" s="15">
+        <f t="shared" si="8"/>
+        <v>0.34339721219614339</v>
+      </c>
+      <c r="V5" s="15">
+        <f t="shared" si="9"/>
+        <v>0.35517276174125223</v>
+      </c>
+      <c r="W5" s="15">
+        <f t="shared" si="10"/>
+        <v>0.30718232503491544</v>
+      </c>
+      <c r="X5" s="15">
+        <f t="shared" si="11"/>
+        <v>0.35038690098955022</v>
+      </c>
+      <c r="Y5" s="15">
+        <f t="shared" si="12"/>
+        <v>0.57802932853100064</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="13"/>
+        <v>-0.36572857087558741</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="0"/>
+        <v>-0.36704610212251959</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="0"/>
+        <v>-0.36765742353895275</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="0"/>
+        <v>-0.36257154198019281</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="0"/>
+        <v>-0.36745680603631009</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="0"/>
+        <v>-0.31683560323945381</v>
+      </c>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="13">
+        <f>SUM(C3:C5)</f>
+        <v>176.8</v>
+      </c>
+      <c r="D6" s="13">
+        <f>SUM(D3:D5)</f>
+        <v>2.5073499999999997</v>
+      </c>
+      <c r="E6" s="13">
+        <f>SUM(E3:E5)</f>
+        <v>7531.9387299999999</v>
+      </c>
+      <c r="F6" s="13">
+        <f>SUM(F3:F5)</f>
+        <v>0.72174400000000005</v>
+      </c>
+      <c r="G6" s="13">
+        <f>SUM(G3:G5)</f>
+        <v>386.97884999999997</v>
+      </c>
+      <c r="H6" s="13">
+        <f>SUM(H3:H5)</f>
+        <v>1.3604500000000002</v>
+      </c>
+      <c r="Z6" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA6" s="19">
+        <f t="shared" ref="AA6:AF6" si="14">SUM(AA3:AA5)</f>
+        <v>-1.0182434088964838</v>
+      </c>
+      <c r="AB6" s="19">
+        <f t="shared" si="14"/>
+        <v>-1.0978756660047577</v>
+      </c>
+      <c r="AC6" s="19">
+        <f t="shared" si="14"/>
+        <v>-1.0864917927960909</v>
+      </c>
+      <c r="AD6" s="19">
+        <f t="shared" si="14"/>
+        <v>-1.0966533037886623</v>
+      </c>
+      <c r="AE6" s="19">
+        <f t="shared" si="14"/>
+        <v>-1.0963448898211903</v>
+      </c>
+      <c r="AF6" s="19">
+        <f t="shared" si="14"/>
+        <v>-0.93620429786544468</v>
+      </c>
+    </row>
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <f>MIN(C3:C5)</f>
+        <v>27.7</v>
+      </c>
+      <c r="D7" s="1">
+        <f>MIN(D3:D5)</f>
+        <v>0.79073099999999996</v>
+      </c>
+      <c r="E7" s="1">
+        <f>MIN(E3:E5)</f>
+        <v>1979.9499499999997</v>
+      </c>
+      <c r="F7" s="1">
+        <f>MIN(F3:F5)</f>
+        <v>0.22170700000000002</v>
+      </c>
+      <c r="G7" s="1">
+        <f>MIN(G3:G5)</f>
+        <v>116.82447999999999</v>
+      </c>
+      <c r="H7" s="1">
+        <f>MIN(H3:H5)</f>
+        <v>0.16831000000000002</v>
+      </c>
+      <c r="Z7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA7" s="21">
+        <f>AA6*(-$AB$1)</f>
+        <v>0.92684509303180984</v>
+      </c>
+      <c r="AB7" s="21">
+        <f t="shared" ref="AB7:AF7" si="15">AB6*(-$AB$1)</f>
+        <v>0.99932949715659458</v>
+      </c>
+      <c r="AC7" s="21">
+        <f t="shared" si="15"/>
+        <v>0.98896744921111968</v>
+      </c>
+      <c r="AD7" s="21">
+        <f t="shared" si="15"/>
+        <v>0.99821685511835812</v>
+      </c>
+      <c r="AE7" s="21">
+        <f t="shared" si="15"/>
+        <v>0.99793612462712544</v>
+      </c>
+      <c r="AF7" s="21">
+        <f t="shared" si="15"/>
+        <v>0.8521698760537636</v>
+      </c>
+    </row>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1">
+        <f>MAX(C3:C5)</f>
+        <v>76.900000000000006</v>
+      </c>
+      <c r="D8" s="1">
+        <f>MAX(D3:D5)</f>
+        <v>0.86101700000000003</v>
+      </c>
+      <c r="E8" s="1">
+        <f>MAX(E3:E5)</f>
+        <v>2876.8493000000003</v>
+      </c>
+      <c r="F8" s="1">
+        <f>MAX(F3:F5)</f>
+        <v>0.25850200000000001</v>
+      </c>
+      <c r="G8" s="1">
+        <f>MAX(G3:G5)</f>
+        <v>135.59232</v>
+      </c>
+      <c r="H8" s="1">
+        <f>MAX(H3:H5)</f>
+        <v>0.78637999999999997</v>
+      </c>
+      <c r="Z8" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA8">
+        <f>$AD$1-AA7</f>
+        <v>7.3154906968190159E-2</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" ref="AB8:AF8" si="16">$AD$1-AB7</f>
+        <v>6.7050284340541833E-4</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="16"/>
+        <v>1.1032550788880324E-2</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="16"/>
+        <v>1.7831448816418849E-3</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="16"/>
+        <v>2.0638753728745574E-3</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="16"/>
+        <v>0.1478301239462364</v>
+      </c>
+      <c r="AG8" s="21">
+        <f>SUM(AA8:AF8)</f>
+        <v>0.23653510480122875</v>
+      </c>
+      <c r="AH8">
+        <v>0.23653510480122875</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="Z9" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA9" s="24">
+        <f>AA8/$AH$8</f>
+        <v>0.30927716640481578</v>
+      </c>
+      <c r="AB9" s="24">
+        <f t="shared" ref="AB9:AF9" si="17">AB8/$AH$8</f>
+        <v>2.8346863945158266E-3</v>
+      </c>
+      <c r="AC9" s="24">
+        <f t="shared" si="17"/>
+        <v>4.6642340037228218E-2</v>
+      </c>
+      <c r="AD9" s="24">
+        <f t="shared" si="17"/>
+        <v>7.5386056676041511E-3</v>
+      </c>
+      <c r="AE9" s="24">
+        <f t="shared" si="17"/>
+        <v>8.7254506032367844E-3</v>
+      </c>
+      <c r="AF9" s="24">
+        <f t="shared" si="17"/>
+        <v>0.62498175089259922</v>
+      </c>
+      <c r="AG9" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="N3:N5 K3:K5" formula="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Experiments of Case Study Finished
</commit_message>
<xml_diff>
--- a/Case study/Num Res.xlsx
+++ b/Case study/Num Res.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inosoft_04\Desktop\PAPER\MATLAB\CASE STUDY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A574467B-492E-4CC1-B6FF-64A98D85AD4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF2AC4B-B6C4-4D1D-AE16-B9ED7052FA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{D6129A20-1F81-494B-BF6B-C0ED5DF90618}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{D6129A20-1F81-494B-BF6B-C0ED5DF90618}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -250,10 +250,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA82E70-FE4C-4668-AB26-ACA18349451D}">
   <dimension ref="A1:AE12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,37 +610,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="G1" s="20" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="Q1" s="19" t="s">
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="Q1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
       <c r="V1" s="20" t="s">
         <v>6</v>
       </c>
       <c r="W1" s="20"/>
       <c r="X1" s="20"/>
-      <c r="AA1" s="19" t="s">
+      <c r="AA1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AE1" s="18" t="s">
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AE1" s="19" t="s">
         <v>9</v>
       </c>
     </row>
@@ -702,7 +702,7 @@
       <c r="AC2" s="1">
         <v>1</v>
       </c>
-      <c r="AE2" s="18"/>
+      <c r="AE2" s="19"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -762,7 +762,7 @@
       <c r="AC3" s="1">
         <v>1</v>
       </c>
-      <c r="AE3" s="18"/>
+      <c r="AE3" s="19"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -822,7 +822,7 @@
       <c r="AC4" s="1">
         <v>1</v>
       </c>
-      <c r="AE4" s="18"/>
+      <c r="AE4" s="19"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -882,7 +882,7 @@
       <c r="AC5" s="1">
         <v>1</v>
       </c>
-      <c r="AE5" s="18"/>
+      <c r="AE5" s="19"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -942,7 +942,7 @@
       <c r="AC6" s="1">
         <v>1</v>
       </c>
-      <c r="AE6" s="18"/>
+      <c r="AE6" s="19"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1002,7 +1002,7 @@
       <c r="AC7" s="1">
         <v>1</v>
       </c>
-      <c r="AE7" s="18"/>
+      <c r="AE7" s="19"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1062,7 +1062,7 @@
       <c r="AC8" s="1">
         <v>1</v>
       </c>
-      <c r="AE8" s="18"/>
+      <c r="AE8" s="19"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1074,31 +1074,55 @@
       <c r="C9" s="1">
         <v>26</v>
       </c>
+      <c r="D9" s="1">
+        <v>93</v>
+      </c>
       <c r="G9" s="1">
         <v>0.82174000000000003</v>
       </c>
       <c r="H9" s="1">
         <v>0.77508999999999995</v>
       </c>
+      <c r="I9" s="1">
+        <v>0.57889999999999997</v>
+      </c>
       <c r="L9" s="1">
         <v>1839.3648000000001</v>
       </c>
       <c r="M9" s="1">
         <v>1632.8586</v>
       </c>
+      <c r="N9" s="1">
+        <v>5449.2502999999997</v>
+      </c>
       <c r="Q9" s="1">
         <v>0.31225999999999998</v>
       </c>
       <c r="R9" s="1">
         <v>0.28226000000000001</v>
       </c>
+      <c r="S9" s="1">
+        <v>0.20899999999999999</v>
+      </c>
       <c r="V9" s="1">
         <v>136.57220000000001</v>
       </c>
       <c r="W9" s="1">
         <v>128.9699</v>
       </c>
-      <c r="AE9" s="18"/>
+      <c r="X9" s="1">
+        <v>107.1152</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>9.0899999999999995E-2</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="19"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1110,31 +1134,55 @@
       <c r="C10" s="1">
         <v>26</v>
       </c>
+      <c r="D10" s="1">
+        <v>68</v>
+      </c>
       <c r="G10" s="1">
         <v>0.84157000000000004</v>
       </c>
       <c r="H10" s="1">
         <v>0.91464999999999996</v>
       </c>
+      <c r="I10" s="1">
+        <v>0.90349999999999997</v>
+      </c>
       <c r="L10" s="1">
         <v>2460.1030000000001</v>
       </c>
       <c r="M10" s="1">
         <v>1801.0408</v>
       </c>
+      <c r="N10" s="1">
+        <v>3799.5549999999998</v>
+      </c>
       <c r="Q10" s="1">
         <v>0.28037000000000001</v>
       </c>
       <c r="R10" s="1">
         <v>0.17019999999999999</v>
       </c>
+      <c r="S10" s="1">
+        <v>0.16400000000000001</v>
+      </c>
       <c r="V10" s="1">
         <v>134.86019999999999</v>
       </c>
       <c r="W10" s="1">
         <v>121.7064</v>
       </c>
-      <c r="AE10" s="18"/>
+      <c r="X10" s="1">
+        <v>140.5213</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="19"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1146,31 +1194,55 @@
       <c r="C11" s="1">
         <v>29</v>
       </c>
+      <c r="D11" s="1">
+        <v>135</v>
+      </c>
       <c r="G11" s="1">
         <v>0.82396999999999998</v>
       </c>
       <c r="H11" s="1">
         <v>0.88934999999999997</v>
       </c>
+      <c r="I11" s="1">
+        <v>0.86160000000000003</v>
+      </c>
       <c r="L11" s="1">
         <v>2191.8798999999999</v>
       </c>
       <c r="M11" s="1">
         <v>3154.1939000000002</v>
       </c>
+      <c r="N11" s="1">
+        <v>3186.0774999999999</v>
+      </c>
       <c r="Q11" s="1">
         <v>0.19599</v>
       </c>
       <c r="R11" s="1">
         <v>0.24364</v>
       </c>
+      <c r="S11" s="1">
+        <v>0.26440000000000002</v>
+      </c>
       <c r="V11" s="1">
         <v>134.6978</v>
       </c>
       <c r="W11" s="1">
         <v>119.35169999999999</v>
       </c>
-      <c r="AE11" s="18"/>
+      <c r="X11" s="1">
+        <v>175.23570000000001</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="19"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
@@ -1183,7 +1255,7 @@
       </c>
       <c r="D12" s="5">
         <f t="shared" si="0"/>
-        <v>67.3</v>
+        <v>96.9</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="5">
@@ -1196,7 +1268,7 @@
       </c>
       <c r="I12" s="5">
         <f t="shared" si="0"/>
-        <v>0.50612000000000001</v>
+        <v>0.74052000000000007</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="5">
@@ -1209,7 +1281,7 @@
       </c>
       <c r="N12" s="5">
         <f t="shared" si="0"/>
-        <v>3363.26109</v>
+        <v>4606.7493699999995</v>
       </c>
       <c r="P12" s="1"/>
       <c r="Q12" s="5">
@@ -1222,7 +1294,7 @@
       </c>
       <c r="S12" s="5">
         <f t="shared" si="0"/>
-        <v>0.14552999999999999</v>
+        <v>0.20927000000000001</v>
       </c>
       <c r="U12" s="1"/>
       <c r="V12" s="5">
@@ -1235,12 +1307,12 @@
       </c>
       <c r="X12" s="5">
         <f t="shared" si="0"/>
-        <v>91.191420000000008</v>
+        <v>133.47863999999998</v>
       </c>
       <c r="Z12" s="1"/>
       <c r="AA12" s="5">
         <f t="shared" si="0"/>
-        <v>4.5400000000000006E-3</v>
+        <v>1.363E-2</v>
       </c>
       <c r="AB12" s="5">
         <f t="shared" si="0"/>
@@ -1248,7 +1320,7 @@
       </c>
       <c r="AC12" s="5">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1270,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB4218F-2606-4969-8B7B-6617CAB0479F}">
   <dimension ref="B1:AH9"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,19 +1466,19 @@
         <v>134.56205</v>
       </c>
       <c r="H3" s="1">
-        <v>0.40576000000000001</v>
+        <v>1.363E-2</v>
       </c>
       <c r="J3" s="1">
         <f>(C3-C$7)/(C$8-C$7)</f>
-        <v>1</v>
+        <v>0.71098265895953761</v>
       </c>
       <c r="K3" s="1">
         <f>(D$8-D3)/(D$8-D$7)</f>
-        <v>1</v>
+        <v>0.56369371404737545</v>
       </c>
       <c r="L3" s="1">
         <f>(E3-E$7)/(E$8-E$7)</f>
-        <v>1</v>
+        <v>0.34144188672007575</v>
       </c>
       <c r="M3" s="1">
         <f>(F3-F$7)/(F$8-F$7)</f>
@@ -1414,66 +1486,66 @@
       </c>
       <c r="N3" s="1">
         <f>(G$8-G3)/(G$8-G$7)</f>
-        <v>5.4895502092942035E-2</v>
+        <v>0</v>
       </c>
       <c r="O3" s="1">
         <f>(H3-H$7)/(H$8-H$7)</f>
-        <v>0.38417978546119375</v>
+        <v>1.3531353135313532E-2</v>
       </c>
       <c r="Q3" s="1">
         <f>SQRT(J3+K3^2+L3+M3+N3^2+O3^2)</f>
-        <v>2.0373040086612124</v>
+        <v>1.5395967804765669</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="T3" s="8">
         <f>C3/$C$6</f>
-        <v>0.43495475113122173</v>
+        <v>0.38163771712158812</v>
       </c>
       <c r="U3" s="8">
         <f>D3/$D$6</f>
-        <v>0.31536522623486951</v>
+        <v>0.33128600713994538</v>
       </c>
       <c r="V3" s="8">
         <f>E3/$E$6</f>
-        <v>0.38195335930461033</v>
+        <v>0.30399265809446441</v>
       </c>
       <c r="W3" s="8">
         <f>F3/$F$6</f>
-        <v>0.35816300516526633</v>
+        <v>0.3644430408835666</v>
       </c>
       <c r="X3" s="8">
         <f>G3/$G$6</f>
-        <v>0.34772455910704164</v>
+        <v>0.34963426282508236</v>
       </c>
       <c r="Y3" s="8">
         <f>H3/$H$6</f>
-        <v>0.29825425410709688</v>
+        <v>1.3445394730352262E-2</v>
       </c>
       <c r="AA3">
         <f>T3*LN(T3)</f>
-        <v>-0.36210560377211848</v>
+        <v>-0.36762531774143037</v>
       </c>
       <c r="AB3">
         <f t="shared" ref="AB3:AF5" si="0">U3*LN(U3)</f>
-        <v>-0.36393899677198266</v>
+        <v>-0.36599590447244484</v>
       </c>
       <c r="AC3">
         <f t="shared" si="0"/>
-        <v>-0.36761359797319193</v>
+        <v>-0.36197978319056273</v>
       </c>
       <c r="AD3">
         <f t="shared" si="0"/>
-        <v>-0.36774998101419282</v>
+        <v>-0.36786334107513613</v>
       </c>
       <c r="AE3">
         <f t="shared" si="0"/>
-        <v>-0.36731696357758076</v>
+        <v>-0.3674193306139058</v>
       </c>
       <c r="AF3">
         <f t="shared" si="0"/>
-        <v>-0.36083066734982788</v>
+        <v>-5.7937800930975426E-2</v>
       </c>
     </row>
     <row r="4" spans="2:34" x14ac:dyDescent="0.25">
@@ -1496,7 +1568,7 @@
         <v>116.82447999999999</v>
       </c>
       <c r="H4" s="1">
-        <v>0.16831000000000002</v>
+        <v>1E-4</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" ref="J4:J5" si="1">(C4-C$7)/(C$8-C$7)</f>
@@ -1504,7 +1576,7 @@
       </c>
       <c r="K4" s="1">
         <f t="shared" ref="K4:K5" si="2">(D$8-D4)/(D$8-D$7)</f>
-        <v>7.7042369746465209E-2</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" ref="L4:M5" si="3">(E4-E$7)/(E$8-E$7)</f>
@@ -1512,7 +1584,7 @@
       </c>
       <c r="M4" s="1">
         <f t="shared" si="3"/>
-        <v>0.53887756488653316</v>
+        <v>0.65536642833929126</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" ref="N4:N5" si="4">(G$8-G4)/(G$8-G$7)</f>
@@ -1524,58 +1596,58 @@
       </c>
       <c r="Q4" s="1">
         <f t="shared" ref="Q4:Q5" si="6">SQRT(J4+K4^2+L4+M4+N4^2+O4^2)</f>
-        <v>1.242905101615841</v>
+        <v>1.2866104415631374</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="T4" s="8">
         <f t="shared" ref="T4:T5" si="7">C4/$C$6</f>
-        <v>0.15667420814479638</v>
+        <v>0.13746898263027296</v>
       </c>
       <c r="U4" s="8">
         <f t="shared" ref="U4:U5" si="8">D4/$D$6</f>
-        <v>0.34123756156898721</v>
+        <v>0.35846447183802271</v>
       </c>
       <c r="V4" s="8">
         <f t="shared" ref="V4:V5" si="9">E4/$E$6</f>
-        <v>0.26287387895413744</v>
+        <v>0.20921855315622606</v>
       </c>
       <c r="W4" s="8">
         <f t="shared" ref="W4:W5" si="10">F4/$F$6</f>
-        <v>0.33465466979981817</v>
+        <v>0.34052250999919631</v>
       </c>
       <c r="X4" s="8">
         <f t="shared" ref="X4:X5" si="11">G4/$G$6</f>
-        <v>0.30188853990340819</v>
+        <v>0.30354651214605882</v>
       </c>
       <c r="Y4" s="8">
         <f t="shared" ref="Y4:Y5" si="12">H4/$H$6</f>
-        <v>0.12371641736190231</v>
+        <v>9.8645595967368041E-5</v>
       </c>
       <c r="AA4">
         <f t="shared" ref="AA4:AA5" si="13">T4*LN(T4)</f>
-        <v>-0.2904092342487779</v>
+        <v>-0.2727875335928458</v>
       </c>
       <c r="AB4">
         <f t="shared" si="0"/>
-        <v>-0.36689056711025547</v>
+        <v>-0.3677579235580527</v>
       </c>
       <c r="AC4">
         <f t="shared" si="0"/>
-        <v>-0.35122077128394619</v>
+        <v>-0.32729645496499482</v>
       </c>
       <c r="AD4">
         <f t="shared" si="0"/>
-        <v>-0.3663317807942767</v>
+        <v>-0.36683606241292427</v>
       </c>
       <c r="AE4">
         <f t="shared" si="0"/>
-        <v>-0.36157112020729937</v>
+        <v>-0.36189435253276037</v>
       </c>
       <c r="AF4">
         <f t="shared" si="0"/>
-        <v>-0.25853802727616293</v>
+        <v>-9.0990470534551518E-4</v>
       </c>
     </row>
     <row r="5" spans="2:34" x14ac:dyDescent="0.25">
@@ -1583,34 +1655,34 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>72.2</v>
+        <v>96.9</v>
       </c>
       <c r="D5" s="1">
-        <v>0.86101700000000003</v>
+        <v>0.74052000000000007</v>
       </c>
       <c r="E5" s="1">
-        <v>2675.1394799999998</v>
+        <v>4606.7493699999995</v>
       </c>
       <c r="F5" s="1">
-        <v>0.22170700000000002</v>
+        <v>0.20927000000000001</v>
       </c>
       <c r="G5" s="1">
-        <v>135.59232</v>
+        <v>133.47863999999998</v>
       </c>
       <c r="H5" s="1">
-        <v>0.78637999999999997</v>
+        <v>1</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" si="1"/>
-        <v>0.90447154471544711</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="3"/>
-        <v>0.77510317071809631</v>
+        <v>1</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="3"/>
@@ -1618,7 +1690,7 @@
       </c>
       <c r="N5" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.1079956273605379E-2</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" si="5"/>
@@ -1626,58 +1698,58 @@
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="6"/>
-        <v>1.6369406572730556</v>
+        <v>2.0009324728881746</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T5" s="8">
         <f t="shared" si="7"/>
-        <v>0.40837104072398189</v>
+        <v>0.48089330024813898</v>
       </c>
       <c r="U5" s="8">
         <f t="shared" si="8"/>
-        <v>0.34339721219614339</v>
+        <v>0.31024952102203196</v>
       </c>
       <c r="V5" s="8">
         <f t="shared" si="9"/>
-        <v>0.35517276174125223</v>
+        <v>0.48678878874930953</v>
       </c>
       <c r="W5" s="8">
         <f t="shared" si="10"/>
-        <v>0.30718232503491544</v>
+        <v>0.29503444911723692</v>
       </c>
       <c r="X5" s="8">
         <f t="shared" si="11"/>
-        <v>0.35038690098955022</v>
+        <v>0.34681922502885881</v>
       </c>
       <c r="Y5" s="8">
         <f t="shared" si="12"/>
-        <v>0.57802932853100064</v>
+        <v>0.98645595967368038</v>
       </c>
       <c r="AA5">
         <f t="shared" si="13"/>
-        <v>-0.36572857087558741</v>
+        <v>-0.35206672791703553</v>
       </c>
       <c r="AB5">
         <f t="shared" si="0"/>
-        <v>-0.36704610212251959</v>
+        <v>-0.36310933762479519</v>
       </c>
       <c r="AC5">
         <f t="shared" si="0"/>
-        <v>-0.36765742353895275</v>
+        <v>-0.35045139373923007</v>
       </c>
       <c r="AD5">
         <f t="shared" si="0"/>
-        <v>-0.36257154198019281</v>
+        <v>-0.36013768084157394</v>
       </c>
       <c r="AE5">
         <f t="shared" si="0"/>
-        <v>-0.36745680603631009</v>
+        <v>-0.36726477329653856</v>
       </c>
       <c r="AF5">
         <f t="shared" si="0"/>
-        <v>-0.31683560323945381</v>
+        <v>-1.3451902896144584E-2</v>
       </c>
     </row>
     <row r="6" spans="2:34" x14ac:dyDescent="0.25">
@@ -1686,54 +1758,54 @@
       </c>
       <c r="C6" s="6">
         <f t="shared" ref="C6:H6" si="14">SUM(C3:C5)</f>
-        <v>176.8</v>
+        <v>201.5</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="14"/>
-        <v>2.5073499999999997</v>
+        <v>2.3868529999999999</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" si="14"/>
-        <v>7531.9387299999999</v>
+        <v>9463.5486199999996</v>
       </c>
       <c r="F6" s="6">
         <f t="shared" si="14"/>
-        <v>0.72174400000000005</v>
+        <v>0.70930700000000013</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" si="14"/>
-        <v>386.97884999999997</v>
+        <v>384.86516999999998</v>
       </c>
       <c r="H6" s="6">
         <f t="shared" si="14"/>
-        <v>1.3604500000000002</v>
+        <v>1.01373</v>
       </c>
       <c r="Z6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="AA6" s="12">
         <f t="shared" ref="AA6:AF6" si="15">SUM(AA3:AA5)</f>
-        <v>-1.0182434088964838</v>
+        <v>-0.99247957925131169</v>
       </c>
       <c r="AB6" s="12">
         <f t="shared" si="15"/>
-        <v>-1.0978756660047577</v>
+        <v>-1.0968631656552927</v>
       </c>
       <c r="AC6" s="12">
         <f t="shared" si="15"/>
-        <v>-1.0864917927960909</v>
+        <v>-1.0397276318947877</v>
       </c>
       <c r="AD6" s="12">
         <f t="shared" si="15"/>
-        <v>-1.0966533037886623</v>
+        <v>-1.0948370843296344</v>
       </c>
       <c r="AE6" s="12">
         <f t="shared" si="15"/>
-        <v>-1.0963448898211903</v>
+        <v>-1.0965784564432048</v>
       </c>
       <c r="AF6" s="12">
         <f t="shared" si="15"/>
-        <v>-0.93620429786544468</v>
+        <v>-7.2299608532465531E-2</v>
       </c>
     </row>
     <row r="7" spans="2:34" x14ac:dyDescent="0.25">
@@ -1746,7 +1818,7 @@
       </c>
       <c r="D7" s="1">
         <f t="shared" si="16"/>
-        <v>0.79073099999999996</v>
+        <v>0.74052000000000007</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="16"/>
@@ -1754,7 +1826,7 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" si="16"/>
-        <v>0.22170700000000002</v>
+        <v>0.20927000000000001</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="16"/>
@@ -1762,34 +1834,34 @@
       </c>
       <c r="H7" s="1">
         <f t="shared" si="16"/>
-        <v>0.16831000000000002</v>
+        <v>1E-4</v>
       </c>
       <c r="Z7" s="13" t="s">
         <v>21</v>
       </c>
       <c r="AA7" s="14">
         <f>AA6*(-$AB$1)</f>
-        <v>0.92684509303180984</v>
+        <v>0.90339384466064288</v>
       </c>
       <c r="AB7" s="14">
         <f t="shared" ref="AB7:AF7" si="17">AB6*(-$AB$1)</f>
-        <v>0.99932949715659458</v>
+        <v>0.99840787962153821</v>
       </c>
       <c r="AC7" s="14">
         <f t="shared" si="17"/>
-        <v>0.98896744921111968</v>
+        <v>0.94640087555846453</v>
       </c>
       <c r="AD7" s="14">
         <f t="shared" si="17"/>
-        <v>0.99821685511835812</v>
+        <v>0.99656366092258797</v>
       </c>
       <c r="AE7" s="14">
         <f t="shared" si="17"/>
-        <v>0.99793612462712544</v>
+        <v>0.9981487261285138</v>
       </c>
       <c r="AF7" s="14">
         <f t="shared" si="17"/>
-        <v>0.8521698760537636</v>
+        <v>6.5809939756014513E-2</v>
       </c>
     </row>
     <row r="8" spans="2:34" x14ac:dyDescent="0.25">
@@ -1798,15 +1870,15 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" ref="C8:H8" si="18">MAX(C3:C5)</f>
-        <v>76.900000000000006</v>
+        <v>96.9</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="18"/>
-        <v>0.86101700000000003</v>
+        <v>0.85560199999999997</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="18"/>
-        <v>2876.8493000000003</v>
+        <v>4606.7493699999995</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="18"/>
@@ -1814,45 +1886,45 @@
       </c>
       <c r="G8" s="1">
         <f t="shared" si="18"/>
-        <v>135.59232</v>
+        <v>134.56205</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="18"/>
-        <v>0.78637999999999997</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="15" t="s">
         <v>22</v>
       </c>
       <c r="AA8">
         <f>$AD$1-AA7</f>
-        <v>7.3154906968190159E-2</v>
+        <v>9.6606155339357125E-2</v>
       </c>
       <c r="AB8">
         <f t="shared" ref="AB8:AF8" si="19">$AD$1-AB7</f>
-        <v>6.7050284340541833E-4</v>
+        <v>1.5921203784617921E-3</v>
       </c>
       <c r="AC8">
         <f t="shared" si="19"/>
-        <v>1.1032550788880324E-2</v>
+        <v>5.3599124441535473E-2</v>
       </c>
       <c r="AD8">
         <f t="shared" si="19"/>
-        <v>1.7831448816418849E-3</v>
+        <v>3.4363390774120317E-3</v>
       </c>
       <c r="AE8">
         <f t="shared" si="19"/>
-        <v>2.0638753728745574E-3</v>
+        <v>1.8512738714862031E-3</v>
       </c>
       <c r="AF8">
         <f t="shared" si="19"/>
-        <v>0.1478301239462364</v>
+        <v>0.93419006024398543</v>
       </c>
       <c r="AG8" s="14">
         <f>SUM(AA8:AF8)</f>
-        <v>0.23653510480122875</v>
+        <v>1.0912750733522381</v>
       </c>
       <c r="AH8">
-        <v>0.23653510480122875</v>
+        <v>1.0912750733522381</v>
       </c>
     </row>
     <row r="9" spans="2:34" x14ac:dyDescent="0.25">
@@ -1861,27 +1933,27 @@
       </c>
       <c r="AA9" s="17">
         <f>AA8/$AH$8</f>
-        <v>0.30927716640481578</v>
+        <v>8.8525943365128909E-2</v>
       </c>
       <c r="AB9" s="17">
         <f t="shared" ref="AB9:AF9" si="20">AB8/$AH$8</f>
-        <v>2.8346863945158266E-3</v>
+        <v>1.4589542245943823E-3</v>
       </c>
       <c r="AC9" s="17">
         <f t="shared" si="20"/>
-        <v>4.6642340037228218E-2</v>
+        <v>4.9116053092724613E-2</v>
       </c>
       <c r="AD9" s="17">
         <f t="shared" si="20"/>
-        <v>7.5386056676041511E-3</v>
+        <v>3.1489210752849864E-3</v>
       </c>
       <c r="AE9" s="17">
         <f t="shared" si="20"/>
-        <v>8.7254506032367844E-3</v>
+        <v>1.6964319232541064E-3</v>
       </c>
       <c r="AF9" s="17">
         <f t="shared" si="20"/>
-        <v>0.62498175089259922</v>
+        <v>0.85605369631901296</v>
       </c>
       <c r="AG9" s="14"/>
     </row>

</xml_diff>